<commit_message>
docs(timetracking) : replace Zeitaufzeichnung_Gruendlinger_Diana.xlsx
</commit_message>
<xml_diff>
--- a/docs/timetracking/Zeitaufzeichnung_Gruendlinger_Diana.xlsx
+++ b/docs/timetracking/Zeitaufzeichnung_Gruendlinger_Diana.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
   <si>
     <t xml:space="preserve">Datum</t>
   </si>
@@ -188,7 +188,13 @@
     <t xml:space="preserve">Datenbank mit neuen Kategorien/Begriffen füttern</t>
   </si>
   <si>
-    <t xml:space="preserve">Dokumentation des auftretenden “fatal” Errors</t>
+    <t xml:space="preserve">Dokumentation des auftretenden “fatal errors”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry: Installationsskript (JDK 11 -&gt; kein “fatal error”?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teammeeting: Testdrehbuch</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -451,11 +457,11 @@
   <dimension ref="A1:D1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
-      <selection pane="bottomRight" activeCell="D49" activeCellId="0" sqref="D49"/>
+      <selection pane="bottomLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="D52" activeCellId="0" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1139,19 +1145,46 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="6"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="8"/>
+      <c r="A49" s="1" t="n">
+        <v>44326</v>
+      </c>
+      <c r="B49" s="6" t="n">
+        <v>0.0729166666666667</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="6"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="8"/>
+      <c r="A50" s="1" t="n">
+        <v>44326</v>
+      </c>
+      <c r="B50" s="6" t="n">
+        <v>0.197916666666667</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="6"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="8"/>
+      <c r="A51" s="1" t="n">
+        <v>44328</v>
+      </c>
+      <c r="B51" s="6" t="n">
+        <v>0.15625</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="6"/>
@@ -5943,10 +5976,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5970,7 +6003,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5978,7 +6011,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5986,7 +6019,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
docs(timetracking): final update of Zeitaufzeichnung_Gruendlinger_Diana.xlsx
</commit_message>
<xml_diff>
--- a/docs/timetracking/Zeitaufzeichnung_Gruendlinger_Diana.xlsx
+++ b/docs/timetracking/Zeitaufzeichnung_Gruendlinger_Diana.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="61">
   <si>
     <t xml:space="preserve">Datum</t>
   </si>
@@ -212,16 +212,19 @@
     <t xml:space="preserve">Systemtest</t>
   </si>
   <si>
+    <t xml:space="preserve">Abschlussbericht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abschlusspräsentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planung der Präsentation</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
     <t xml:space="preserve">Bezeichnung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abschlussbericht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abschlusspräsentation</t>
   </si>
 </sst>
 </file>
@@ -234,7 +237,7 @@
     <numFmt numFmtId="166" formatCode="h:mm"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -286,13 +289,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -351,7 +347,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -392,11 +388,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,11 +472,11 @@
   <dimension ref="A1:D1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
-      <selection pane="bottomRight" activeCell="D60" activeCellId="0" sqref="D60"/>
+      <selection pane="bottomLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+      <selection pane="bottomRight" activeCell="D63" activeCellId="0" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1303,7 +1295,7 @@
       <c r="C58" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D58" s="10" t="s">
+      <c r="D58" s="8" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1322,19 +1314,46 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="6"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="8"/>
+      <c r="A60" s="1" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B60" s="6" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="6"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="8"/>
+      <c r="A61" s="1" t="n">
+        <v>44364</v>
+      </c>
+      <c r="B61" s="6" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="6"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="8"/>
+      <c r="A62" s="1" t="n">
+        <v>44364</v>
+      </c>
+      <c r="B62" s="6" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="6"/>
@@ -6070,11 +6089,11 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>57</v>
+      <c r="A1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6106,7 +6125,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6114,7 +6133,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>